<commit_message>
edit data and change log
</commit_message>
<xml_diff>
--- a/Data/Excel Files/All years/edited/change logs/Hakai_change_log.xlsx
+++ b/Data/Excel Files/All years/edited/change logs/Hakai_change_log.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mawha\Dropbox\Martone Lab\martone_calvert\Data\Excel Files\All years\edited\change logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4DFC59-3265-4087-927D-5596692C7A98}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476FEF7C-C406-4CD8-8EB3-E06F12D2328E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13368" xr2:uid="{4E89C64D-041D-4526-88EC-5CB81F9ED7B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Martone Lab Hakai rocky shore seaweed project</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Changed blanks for samplers and recorders to "???"</t>
+  </si>
+  <si>
+    <t>Changed dates from 12 July 2014 to 14 July 2015</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9BFE01-FA11-4C94-A4A2-C3300FE152E1}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,6 +750,20 @@
         <v>28</v>
       </c>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>44701</v>
+      </c>
+      <c r="B22" s="4">
+        <v>2015</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
update raw data for 2022
</commit_message>
<xml_diff>
--- a/Data/Excel Files/All years/edited/change logs/Hakai_change_log.xlsx
+++ b/Data/Excel Files/All years/edited/change logs/Hakai_change_log.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mawha\Dropbox\Martone Lab\martone_calvert\Data\Excel Files\All years\edited\change logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476FEF7C-C406-4CD8-8EB3-E06F12D2328E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC053C45-B29E-4B75-8CE1-E104AEF91EC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13368" xr2:uid="{4E89C64D-041D-4526-88EC-5CB81F9ED7B3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13370" xr2:uid="{4E89C64D-041D-4526-88EC-5CB81F9ED7B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Martone Lab Hakai rocky shore seaweed project</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Changed dates from 12 July 2014 to 14 July 2015</t>
+  </si>
+  <si>
+    <t>Foggy Cove HIGH Quadrat 8</t>
+  </si>
+  <si>
+    <t>Changed barnacle cover from 440% to 44%</t>
   </si>
 </sst>
 </file>
@@ -478,38 +484,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9BFE01-FA11-4C94-A4A2-C3300FE152E1}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -526,7 +532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>43452</v>
       </c>
@@ -540,7 +546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>43452</v>
       </c>
@@ -554,7 +560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>43452</v>
       </c>
@@ -568,7 +574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>43452</v>
       </c>
@@ -582,7 +588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>43452</v>
       </c>
@@ -599,7 +605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>43452</v>
       </c>
@@ -613,7 +619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>43452</v>
       </c>
@@ -627,7 +633,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>43453</v>
       </c>
@@ -641,7 +647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>43454</v>
       </c>
@@ -655,7 +661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>43454</v>
       </c>
@@ -669,7 +675,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>43454</v>
       </c>
@@ -683,7 +689,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>43454</v>
       </c>
@@ -697,7 +703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>43454</v>
       </c>
@@ -711,7 +717,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>43454</v>
       </c>
@@ -722,7 +728,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>43455</v>
       </c>
@@ -736,7 +742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>43494</v>
       </c>
@@ -750,7 +756,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>44701</v>
       </c>
@@ -762,6 +768,20 @@
       </c>
       <c r="D22" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>44766</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2022</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>